<commit_message>
Update scripts and data used in model
</commit_message>
<xml_diff>
--- a/csse_covid_19_data/csse_covid_19_daily_reports_us/StatesinFitting.xlsx
+++ b/csse_covid_19_data/csse_covid_19_daily_reports_us/StatesinFitting.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chadr\Desktop\COVID-19_Data\csse_covid_19_data\csse_covid_19_daily_reports_us\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B50405A9-A9B8-4F4D-B36C-63D1F8BF8733}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F128F64-FC60-4011-9388-6B9B483050D9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="4215" windowWidth="21600" windowHeight="11385" xr2:uid="{3A4C624D-2EF0-439E-806B-0CD50B6790E0}"/>
+    <workbookView xWindow="0" yWindow="3330" windowWidth="21600" windowHeight="11385" xr2:uid="{B4A3A41F-EE6B-4C1D-9588-91F4518641D5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,57 +33,99 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+  <si>
+    <t>Colorado</t>
+  </si>
   <si>
     <t>CO</t>
   </si>
   <si>
+    <t>Connecticut</t>
+  </si>
+  <si>
     <t>CT</t>
   </si>
   <si>
+    <t>Delaware</t>
+  </si>
+  <si>
     <t>DE</t>
   </si>
   <si>
+    <t>Georgia</t>
+  </si>
+  <si>
     <t>GA</t>
   </si>
   <si>
+    <t>Idaho</t>
+  </si>
+  <si>
     <t>ID</t>
   </si>
   <si>
+    <t>Indiana</t>
+  </si>
+  <si>
     <t>IN</t>
   </si>
   <si>
-    <t>KS</t>
-  </si>
-  <si>
-    <t>KY</t>
+    <t>Louisiana</t>
   </si>
   <si>
     <t>LA</t>
   </si>
   <si>
-    <t>MD</t>
-  </si>
-  <si>
-    <t>MI</t>
+    <t>Massachusetts</t>
+  </si>
+  <si>
+    <t>MA</t>
+  </si>
+  <si>
+    <t>Missouri</t>
+  </si>
+  <si>
+    <t>MO</t>
+  </si>
+  <si>
+    <t>New Jersey</t>
   </si>
   <si>
     <t>NJ</t>
   </si>
   <si>
+    <t>New York</t>
+  </si>
+  <si>
     <t>NY</t>
   </si>
   <si>
+    <t>Ohio</t>
+  </si>
+  <si>
     <t>OH</t>
   </si>
   <si>
+    <t>Pennsylvania</t>
+  </si>
+  <si>
     <t>PA</t>
   </si>
   <si>
+    <t>Rhode Island</t>
+  </si>
+  <si>
     <t>RI</t>
   </si>
   <si>
+    <t>Vermont</t>
+  </si>
+  <si>
     <t>VT</t>
+  </si>
+  <si>
+    <t>Washington</t>
   </si>
   <si>
     <t>WA</t>
@@ -437,69 +479,141 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3CEFB15-34EF-4DA1-8CD2-D21B6D2595A0}">
-  <dimension ref="A1:R1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FF3FADC-47E3-4946-9A0E-A125F543BFC6}">
+  <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:R1"/>
+      <selection sqref="A1:B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="B2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="B3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="B4" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="B5" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="B6" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="B7" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>14</v>
       </c>
-      <c r="P1" t="s">
+      <c r="B8" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" t="s">
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>16</v>
       </c>
-      <c r="R1" t="s">
+      <c r="B9" t="s">
         <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>